<commit_message>
Korean -한국어(대한민국) Config Added
</commit_message>
<xml_diff>
--- a/Config/KO/ReportTemplate.xlsx
+++ b/Config/KO/ReportTemplate.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76501EC-82F4-4543-BF55-9F64F492A129}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9E974D-C2BA-4D52-A637-28F01209E511}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="948" yWindow="0" windowWidth="17400" windowHeight="11964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,27 +22,27 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Workflow Filename</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Internal Path</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Suggestion</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Issue</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Target</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Action</t>
+    <t>워크플로우 이름</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>내부 경로</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>대상</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>이슈</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>조치</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>제안</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -50,17 +50,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Yu Gothic"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Yu Gothic"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -90,7 +90,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -109,12 +109,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{151AC480-3815-49A6-B161-4F094CB6C6F9}" name="テーブル1" displayName="テーブル1" ref="A1:F2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="A1:F2" xr:uid="{96568595-11FA-4665-A7F5-5DAA0257F387}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{2633DBB4-FC06-45DE-B4B7-612ADA86082E}" name="Workflow Filename"/>
-    <tableColumn id="2" xr3:uid="{DB7747F9-D92B-4CC1-AB9E-7AE69ADF34C2}" name="Internal Path"/>
-    <tableColumn id="3" xr3:uid="{3B498D3F-8398-47B2-ACE5-B119F71EB4E8}" name="Target"/>
-    <tableColumn id="4" xr3:uid="{A0581726-DF95-4DB9-BDDE-2D527D8D8BB3}" name="Issue"/>
-    <tableColumn id="6" xr3:uid="{F5FBCE47-2F6A-4F15-B22D-7EF25F28710A}" name="Action"/>
-    <tableColumn id="5" xr3:uid="{B19192A5-5CE8-4EE7-A9B5-D071ADEE6AB3}" name="Suggestion"/>
+    <tableColumn id="1" xr3:uid="{2633DBB4-FC06-45DE-B4B7-612ADA86082E}" name="워크플로우 이름"/>
+    <tableColumn id="2" xr3:uid="{DB7747F9-D92B-4CC1-AB9E-7AE69ADF34C2}" name="내부 경로"/>
+    <tableColumn id="3" xr3:uid="{3B498D3F-8398-47B2-ACE5-B119F71EB4E8}" name="대상"/>
+    <tableColumn id="4" xr3:uid="{A0581726-DF95-4DB9-BDDE-2D527D8D8BB3}" name="이슈"/>
+    <tableColumn id="6" xr3:uid="{F5FBCE47-2F6A-4F15-B22D-7EF25F28710A}" name="조치"/>
+    <tableColumn id="5" xr3:uid="{B19192A5-5CE8-4EE7-A9B5-D071ADEE6AB3}" name="제안"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -385,19 +385,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.625" customWidth="1"/>
-    <col min="2" max="2" width="24.75" customWidth="1"/>
-    <col min="3" max="3" width="20.375" customWidth="1"/>
-    <col min="4" max="4" width="36.125" customWidth="1"/>
-    <col min="5" max="5" width="20.625" customWidth="1"/>
-    <col min="6" max="6" width="51.125" customWidth="1"/>
+    <col min="1" max="1" width="19.59765625" customWidth="1"/>
+    <col min="2" max="2" width="24.69921875" customWidth="1"/>
+    <col min="3" max="3" width="20.3984375" customWidth="1"/>
+    <col min="4" max="4" width="36.09765625" customWidth="1"/>
+    <col min="5" max="5" width="20.59765625" customWidth="1"/>
+    <col min="6" max="6" width="51.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -405,16 +407,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>